<commit_message>
manipulate nestle march review
</commit_message>
<xml_diff>
--- a/store_url_mapping.xlsx
+++ b/store_url_mapping.xlsx
@@ -1552,11 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D311"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1589,7 +1588,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1609,7 +1608,7 @@
         <v>4396232</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>4396142</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>3849865</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>4209173</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +1688,7 @@
         <v>5285870</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>4713594</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>4008365</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>4713572</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1769,7 +1768,7 @@
         <v>4712764</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>4712778</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>4007911</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>4712762</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>4712736</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>4007909</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1929,7 +1928,7 @@
         <v>255780</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>1080961</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>25931802723</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1989,7 +1988,7 @@
         <v>25092330368</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2008,7 @@
         <v>25050683515</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>25050683514</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>13695381271</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>13695381267</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>13695381268</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2108,7 @@
         <v>13695381265</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>13695381270</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>13695381262</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>13695381264</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2189,7 +2188,7 @@
         <v>13695381263</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>13695381269</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>13695381266</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>12299826003</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>18555840051</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2289,7 +2288,7 @@
         <v>18555840050</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>12424332573</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2329,7 +2328,7 @@
         <v>16546674330</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2349,7 +2348,7 @@
         <v>16546674329</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>13675223690</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2388,7 @@
         <v>12082162643</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>16545462931</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2429,7 +2428,7 @@
         <v>16545462930</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>16545462929</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2469,7 +2468,7 @@
         <v>12083025102</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2489,7 +2488,7 @@
         <v>16544948616</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2509,7 +2508,7 @@
         <v>16544948617</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2529,7 +2528,7 @@
         <v>13675552365</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>12083146163</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>16498569454</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2588,7 @@
         <v>14446124474</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v>14446124475</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>12400757767</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>12083388599</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>14445404727</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>14445404726</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -2709,7 +2708,7 @@
         <v>13638853955</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2729,7 +2728,7 @@
         <v>12082373228</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2749,7 +2748,7 @@
         <v>14441834226</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>13639679598</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>12298574507</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>13741836484</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2869,7 +2868,7 @@
         <v>13741836486</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>13741836485</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -2909,7 +2908,7 @@
         <v>13674904462</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>13674904461</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -2949,7 +2948,7 @@
         <v>13674728744</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>13674728743</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>13674506362</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +3008,7 @@
         <v>13674506361</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>13674411005</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -3089,7 +3088,7 @@
         <v>13516246557</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -3109,7 +3108,7 @@
         <v>12656575216</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>12656575217</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -3149,7 +3148,7 @@
         <v>12656575218</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>12424200273</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>12539168859</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -3209,7 +3208,7 @@
         <v>12538674481</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>12400682887</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -3249,7 +3248,7 @@
         <v>13467926194</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -3269,7 +3268,7 @@
         <v>12170684578</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -3289,7 +3288,7 @@
         <v>12301482752</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -3309,7 +3308,7 @@
         <v>12301180135</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>12301067262</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -3349,7 +3348,7 @@
         <v>12300597399</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>12300109800</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -3389,7 +3388,7 @@
         <v>12299611125</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -3409,7 +3408,7 @@
         <v>12085074541</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -3429,7 +3428,7 @@
         <v>12082581959</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -3449,7 +3448,7 @@
         <v>1240027</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>4</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>255803</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -3489,7 +3488,7 @@
         <v>255802</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -3509,7 +3508,7 @@
         <v>1240022</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -3529,7 +3528,7 @@
         <v>4857678</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -3549,7 +3548,7 @@
         <v>255797</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>1140667</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>255800</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -3609,7 +3608,7 @@
         <v>4080239</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>255798</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -3649,7 +3648,7 @@
         <v>255799</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -3669,7 +3668,7 @@
         <v>6084935</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>1240023</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -3709,7 +3708,7 @@
         <v>1240024</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -3729,7 +3728,7 @@
         <v>6078298</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>5186742</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>4</v>
       </c>
@@ -3769,7 +3768,7 @@
         <v>1339986</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -3789,7 +3788,7 @@
         <v>1339964</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>1339980</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>1339973</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1">
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>1339960</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1">
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -3869,7 +3868,7 @@
         <v>1339978</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1">
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>4</v>
       </c>
@@ -3889,7 +3888,7 @@
         <v>1339976</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>4</v>
       </c>
@@ -3909,7 +3908,7 @@
         <v>1339992</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>4</v>
       </c>
@@ -3929,7 +3928,7 @@
         <v>1339977</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -3949,7 +3948,7 @@
         <v>1339987</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>1339993</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -3989,7 +3988,7 @@
         <v>1339981</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -4009,7 +4008,7 @@
         <v>1339982</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -4029,7 +4028,7 @@
         <v>1339965</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>4</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>1339983</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>4</v>
       </c>
@@ -4069,7 +4068,7 @@
         <v>1339974</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>4</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>4244687</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>4</v>
       </c>
@@ -4149,7 +4148,7 @@
         <v>102878788</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -4169,7 +4168,7 @@
         <v>610800872</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -4189,7 +4188,7 @@
         <v>610800875</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -4209,7 +4208,7 @@
         <v>103630807</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>610800873</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -4249,7 +4248,7 @@
         <v>610800876</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -4269,7 +4268,7 @@
         <v>610800856</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -4289,7 +4288,7 @@
         <v>610800855</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -4309,7 +4308,7 @@
         <v>610800857</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>610800858</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1">
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>149</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>610800874</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>600017408</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>149</v>
       </c>
@@ -4389,7 +4388,7 @@
         <v>600017407</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -4409,7 +4408,7 @@
         <v>103721215</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1">
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -4429,7 +4428,7 @@
         <v>600017406</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1">
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>149</v>
       </c>
@@ -4449,7 +4448,7 @@
         <v>646949532</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>149</v>
       </c>
@@ -4469,7 +4468,7 @@
         <v>102461581</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1">
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -4489,7 +4488,7 @@
         <v>102461577</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>149</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>123999590</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>102461575</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -4549,7 +4548,7 @@
         <v>120278555</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1">
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -4569,7 +4568,7 @@
         <v>102461579</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -4589,7 +4588,7 @@
         <v>102461576</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>149</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>102461580</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -4629,7 +4628,7 @@
         <v>123996226</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1">
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>149</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>123998119</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1">
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>149</v>
       </c>
@@ -4669,7 +4668,7 @@
         <v>123997670</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1">
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>149</v>
       </c>
@@ -4689,7 +4688,7 @@
         <v>615596524</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1">
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>149</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>781978185</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1">
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>149</v>
       </c>
@@ -4729,7 +4728,7 @@
         <v>615596523</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1">
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>149</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>10092120760</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>149</v>
       </c>
@@ -4769,7 +4768,7 @@
         <v>10092120759</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1">
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>140</v>
       </c>
@@ -4789,7 +4788,7 @@
         <v>533747959004</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1">
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>140</v>
       </c>
@@ -4809,7 +4808,7 @@
         <v>533065312599</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1">
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>140</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>44095998966</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1">
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>140</v>
       </c>
@@ -4849,7 +4848,7 @@
         <v>528373077759</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1">
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>140</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>532732517162</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1">
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>140</v>
       </c>
@@ -4889,7 +4888,7 @@
         <v>40337418469</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1">
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>140</v>
       </c>
@@ -4909,7 +4908,7 @@
         <v>536331066559</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1">
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>140</v>
       </c>
@@ -4929,7 +4928,7 @@
         <v>565044224463</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1">
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>140</v>
       </c>
@@ -4949,7 +4948,7 @@
         <v>23477636937</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1">
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>140</v>
       </c>
@@ -4969,7 +4968,7 @@
         <v>43961411815</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1">
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>140</v>
       </c>
@@ -4989,7 +4988,7 @@
         <v>36130973835</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1">
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>140</v>
       </c>
@@ -5009,7 +5008,7 @@
         <v>524641291671</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1">
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>140</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>23471120077</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1">
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>140</v>
       </c>
@@ -5049,7 +5048,7 @@
         <v>17648438926</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1">
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>140</v>
       </c>
@@ -5069,7 +5068,7 @@
         <v>17648538736</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1">
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>140</v>
       </c>
@@ -5089,7 +5088,7 @@
         <v>19480427581</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1">
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>140</v>
       </c>
@@ -5109,7 +5108,7 @@
         <v>529720140223</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1">
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>140</v>
       </c>
@@ -5129,7 +5128,7 @@
         <v>41205514458</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1">
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>140</v>
       </c>
@@ -5149,7 +5148,7 @@
         <v>41189695491</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1">
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>140</v>
       </c>
@@ -5169,7 +5168,7 @@
         <v>36130743621</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1">
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>140</v>
       </c>
@@ -5189,7 +5188,7 @@
         <v>558429345561</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1">
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>140</v>
       </c>
@@ -5289,7 +5288,7 @@
         <v>39244054131</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1">
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>140</v>
       </c>
@@ -5309,7 +5308,7 @@
         <v>545616955328</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1">
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>140</v>
       </c>
@@ -5329,7 +5328,7 @@
         <v>36984529022</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1">
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>140</v>
       </c>
@@ -5349,7 +5348,7 @@
         <v>23464208294</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1">
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>140</v>
       </c>
@@ -5369,7 +5368,7 @@
         <v>44104247673</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1">
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>140</v>
       </c>
@@ -5389,7 +5388,7 @@
         <v>556392094755</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1">
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>140</v>
       </c>
@@ -5409,7 +5408,7 @@
         <v>39234283947</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1">
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>140</v>
       </c>
@@ -5429,7 +5428,7 @@
         <v>545589366243</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1">
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>140</v>
       </c>
@@ -5449,7 +5448,7 @@
         <v>545135822523</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1">
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>140</v>
       </c>
@@ -5469,7 +5468,7 @@
         <v>544372646926</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1">
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>140</v>
       </c>
@@ -5489,7 +5488,7 @@
         <v>553967190432</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1">
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>140</v>
       </c>
@@ -5509,7 +5508,7 @@
         <v>539966275589</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1">
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>140</v>
       </c>
@@ -5529,7 +5528,7 @@
         <v>539963816913</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1">
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>140</v>
       </c>
@@ -5549,7 +5548,7 @@
         <v>544338112849</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1">
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>140</v>
       </c>
@@ -5569,7 +5568,7 @@
         <v>539966158037</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1">
+    <row r="201" spans="1:6">
       <c r="A201" t="s">
         <v>140</v>
       </c>
@@ -5589,7 +5588,7 @@
         <v>544438110640</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1">
+    <row r="202" spans="1:6">
       <c r="A202" t="s">
         <v>140</v>
       </c>
@@ -5609,7 +5608,7 @@
         <v>539419425366</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1">
+    <row r="203" spans="1:6">
       <c r="A203" t="s">
         <v>140</v>
       </c>
@@ -5629,7 +5628,7 @@
         <v>544390975563</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1">
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
         <v>140</v>
       </c>
@@ -5649,7 +5648,7 @@
         <v>559308160657</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1">
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>140</v>
       </c>
@@ -5669,7 +5668,7 @@
         <v>540012314131</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1">
+    <row r="206" spans="1:6">
       <c r="A206" t="s">
         <v>140</v>
       </c>
@@ -5689,7 +5688,7 @@
         <v>554021827194</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1">
+    <row r="207" spans="1:6">
       <c r="A207" t="s">
         <v>140</v>
       </c>
@@ -5709,7 +5708,7 @@
         <v>545138770586</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1">
+    <row r="208" spans="1:6">
       <c r="A208" t="s">
         <v>140</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>558957811614</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1">
+    <row r="209" spans="1:6">
       <c r="A209" t="s">
         <v>140</v>
       </c>
@@ -5749,7 +5748,7 @@
         <v>558902414522</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1">
+    <row r="210" spans="1:6">
       <c r="A210" t="s">
         <v>140</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>539968095876</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1">
+    <row r="211" spans="1:6">
       <c r="A211" t="s">
         <v>140</v>
       </c>
@@ -5789,7 +5788,7 @@
         <v>553937549311</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1">
+    <row r="212" spans="1:6">
       <c r="A212" t="s">
         <v>140</v>
       </c>
@@ -5809,7 +5808,7 @@
         <v>539966316144</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1">
+    <row r="213" spans="1:6">
       <c r="A213" t="s">
         <v>140</v>
       </c>
@@ -5829,7 +5828,7 @@
         <v>543532688716</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1">
+    <row r="214" spans="1:6">
       <c r="A214" t="s">
         <v>140</v>
       </c>
@@ -5849,7 +5848,7 @@
         <v>539962244112</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1">
+    <row r="215" spans="1:6">
       <c r="A215" t="s">
         <v>140</v>
       </c>
@@ -5869,7 +5868,7 @@
         <v>558950059549</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1">
+    <row r="216" spans="1:6">
       <c r="A216" t="s">
         <v>140</v>
       </c>
@@ -5889,7 +5888,7 @@
         <v>540012726331</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1">
+    <row r="217" spans="1:6">
       <c r="A217" t="s">
         <v>140</v>
       </c>
@@ -5909,7 +5908,7 @@
         <v>540013292848</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1">
+    <row r="218" spans="1:6">
       <c r="A218" t="s">
         <v>140</v>
       </c>
@@ -5929,7 +5928,7 @@
         <v>539966536274</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1">
+    <row r="219" spans="1:6">
       <c r="A219" t="s">
         <v>140</v>
       </c>
@@ -5949,7 +5948,7 @@
         <v>563487222700</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1">
+    <row r="220" spans="1:6">
       <c r="A220" t="s">
         <v>140</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>563418565011</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1">
+    <row r="221" spans="1:6">
       <c r="A221" t="s">
         <v>140</v>
       </c>
@@ -5989,7 +5988,7 @@
         <v>563431853815</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1">
+    <row r="222" spans="1:6">
       <c r="A222" t="s">
         <v>140</v>
       </c>
@@ -6009,7 +6008,7 @@
         <v>563420605298</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1">
+    <row r="223" spans="1:6">
       <c r="A223" t="s">
         <v>140</v>
       </c>
@@ -6029,7 +6028,7 @@
         <v>563419565674</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1">
+    <row r="224" spans="1:6">
       <c r="A224" t="s">
         <v>140</v>
       </c>
@@ -6049,7 +6048,7 @@
         <v>563316704583</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1">
+    <row r="225" spans="1:6">
       <c r="A225" t="s">
         <v>140</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>562946893247</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1">
+    <row r="226" spans="1:6">
       <c r="A226" t="s">
         <v>140</v>
       </c>
@@ -6089,7 +6088,7 @@
         <v>563420381333</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1">
+    <row r="227" spans="1:6">
       <c r="A227" t="s">
         <v>140</v>
       </c>
@@ -6109,7 +6108,7 @@
         <v>563419309173</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1">
+    <row r="228" spans="1:6">
       <c r="A228" t="s">
         <v>140</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>562845712326</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1">
+    <row r="229" spans="1:6">
       <c r="A229" t="s">
         <v>140</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>563090099989</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1">
+    <row r="230" spans="1:6">
       <c r="A230" t="s">
         <v>140</v>
       </c>
@@ -6169,7 +6168,7 @@
         <v>562947573029</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1">
+    <row r="231" spans="1:6">
       <c r="A231" t="s">
         <v>140</v>
       </c>
@@ -6189,7 +6188,7 @@
         <v>563035049517</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1">
+    <row r="232" spans="1:6">
       <c r="A232" t="s">
         <v>140</v>
       </c>
@@ -6209,7 +6208,7 @@
         <v>562933884245</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1">
+    <row r="233" spans="1:6">
       <c r="A233" t="s">
         <v>140</v>
       </c>
@@ -6229,7 +6228,7 @@
         <v>562830496721</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1">
+    <row r="234" spans="1:6">
       <c r="A234" t="s">
         <v>140</v>
       </c>
@@ -6249,7 +6248,7 @@
         <v>563087323512</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1">
+    <row r="235" spans="1:6">
       <c r="A235" t="s">
         <v>140</v>
       </c>
@@ -6269,7 +6268,7 @@
         <v>563008974246</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1">
+    <row r="236" spans="1:6">
       <c r="A236" t="s">
         <v>140</v>
       </c>
@@ -6289,7 +6288,7 @@
         <v>562945937147</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1">
+    <row r="237" spans="1:6">
       <c r="A237" t="s">
         <v>140</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>563088407802</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1">
+    <row r="238" spans="1:6">
       <c r="A238" t="s">
         <v>140</v>
       </c>
@@ -6329,7 +6328,7 @@
         <v>562846656174</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1">
+    <row r="239" spans="1:6">
       <c r="A239" t="s">
         <v>140</v>
       </c>
@@ -6349,7 +6348,7 @@
         <v>563037273548</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1">
+    <row r="240" spans="1:6">
       <c r="A240" t="s">
         <v>140</v>
       </c>
@@ -6369,7 +6368,7 @@
         <v>563414185487</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1">
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
         <v>140</v>
       </c>
@@ -6389,7 +6388,7 @@
         <v>562960624385</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1">
+    <row r="242" spans="1:6">
       <c r="A242" t="s">
         <v>140</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>563494735279</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1">
+    <row r="243" spans="1:6">
       <c r="A243" t="s">
         <v>140</v>
       </c>
@@ -6429,7 +6428,7 @@
         <v>563129262930</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1">
+    <row r="244" spans="1:6">
       <c r="A244" t="s">
         <v>140</v>
       </c>
@@ -6449,7 +6448,7 @@
         <v>563248300822</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1">
+    <row r="245" spans="1:6">
       <c r="A245" t="s">
         <v>140</v>
       </c>
@@ -6469,7 +6468,7 @@
         <v>563248560489</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1">
+    <row r="246" spans="1:6">
       <c r="A246" t="s">
         <v>140</v>
       </c>
@@ -6489,7 +6488,7 @@
         <v>563350305418</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1">
+    <row r="247" spans="1:6">
       <c r="A247" t="s">
         <v>140</v>
       </c>
@@ -6509,7 +6508,7 @@
         <v>563348701369</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1">
+    <row r="248" spans="1:6">
       <c r="A248" t="s">
         <v>140</v>
       </c>
@@ -6529,7 +6528,7 @@
         <v>563351157118</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1">
+    <row r="249" spans="1:6">
       <c r="A249" t="s">
         <v>140</v>
       </c>
@@ -6549,7 +6548,7 @@
         <v>563063461843</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1">
+    <row r="250" spans="1:6">
       <c r="A250" t="s">
         <v>140</v>
       </c>
@@ -6569,7 +6568,7 @@
         <v>563498754207</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1">
+    <row r="251" spans="1:6">
       <c r="A251" t="s">
         <v>140</v>
       </c>
@@ -6589,7 +6588,7 @@
         <v>563328456991</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1">
+    <row r="252" spans="1:6">
       <c r="A252" t="s">
         <v>140</v>
       </c>
@@ -6609,7 +6608,7 @@
         <v>563496502556</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1">
+    <row r="253" spans="1:6">
       <c r="A253" t="s">
         <v>140</v>
       </c>
@@ -6629,7 +6628,7 @@
         <v>564994852144</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1">
+    <row r="254" spans="1:6">
       <c r="A254" t="s">
         <v>140</v>
       </c>
@@ -6649,7 +6648,7 @@
         <v>563071053907</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1">
+    <row r="255" spans="1:6">
       <c r="A255" t="s">
         <v>140</v>
       </c>
@@ -6669,7 +6668,7 @@
         <v>563408758794</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1">
+    <row r="256" spans="1:6">
       <c r="A256" t="s">
         <v>140</v>
       </c>
@@ -6729,7 +6728,7 @@
         <v>523000703198</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1">
+    <row r="259" spans="1:6">
       <c r="A259" t="s">
         <v>140</v>
       </c>
@@ -6749,7 +6748,7 @@
         <v>556308588016</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1">
+    <row r="260" spans="1:6">
       <c r="A260" t="s">
         <v>140</v>
       </c>
@@ -6769,7 +6768,7 @@
         <v>550045667246</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1">
+    <row r="261" spans="1:6">
       <c r="A261" t="s">
         <v>140</v>
       </c>
@@ -6789,7 +6788,7 @@
         <v>550571692826</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1">
+    <row r="262" spans="1:6">
       <c r="A262" t="s">
         <v>140</v>
       </c>
@@ -6809,7 +6808,7 @@
         <v>551519582578</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1">
+    <row r="263" spans="1:6">
       <c r="A263" t="s">
         <v>140</v>
       </c>
@@ -6829,7 +6828,7 @@
         <v>550041691914</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1">
+    <row r="264" spans="1:6">
       <c r="A264" t="s">
         <v>140</v>
       </c>
@@ -6849,7 +6848,7 @@
         <v>549566966809</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1">
+    <row r="265" spans="1:6">
       <c r="A265" t="s">
         <v>140</v>
       </c>
@@ -6869,7 +6868,7 @@
         <v>564878985450</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1">
+    <row r="266" spans="1:6">
       <c r="A266" t="s">
         <v>140</v>
       </c>
@@ -6889,7 +6888,7 @@
         <v>560617745513</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1">
+    <row r="267" spans="1:6">
       <c r="A267" t="s">
         <v>140</v>
       </c>
@@ -6909,7 +6908,7 @@
         <v>551439604956</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1">
+    <row r="268" spans="1:6">
       <c r="A268" t="s">
         <v>140</v>
       </c>
@@ -6929,7 +6928,7 @@
         <v>558695572405</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1">
+    <row r="269" spans="1:6">
       <c r="A269" t="s">
         <v>140</v>
       </c>
@@ -6949,7 +6948,7 @@
         <v>550015274487</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1">
+    <row r="270" spans="1:6">
       <c r="A270" t="s">
         <v>140</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>549985973065</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1">
+    <row r="271" spans="1:6">
       <c r="A271" t="s">
         <v>140</v>
       </c>
@@ -6989,7 +6988,7 @@
         <v>551438024077</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1">
+    <row r="272" spans="1:6">
       <c r="A272" t="s">
         <v>140</v>
       </c>
@@ -7009,7 +7008,7 @@
         <v>549940276744</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1">
+    <row r="273" spans="1:6">
       <c r="A273" t="s">
         <v>140</v>
       </c>
@@ -7029,7 +7028,7 @@
         <v>549989801514</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1">
+    <row r="274" spans="1:6">
       <c r="A274" t="s">
         <v>140</v>
       </c>
@@ -7049,7 +7048,7 @@
         <v>522867607321</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1">
+    <row r="275" spans="1:6">
       <c r="A275" t="s">
         <v>140</v>
       </c>
@@ -7069,7 +7068,7 @@
         <v>550050763816</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1">
+    <row r="276" spans="1:6">
       <c r="A276" t="s">
         <v>140</v>
       </c>
@@ -7089,7 +7088,7 @@
         <v>551525442096</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1">
+    <row r="277" spans="1:6">
       <c r="A277" t="s">
         <v>140</v>
       </c>
@@ -7109,7 +7108,7 @@
         <v>523244710373</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1">
+    <row r="278" spans="1:6">
       <c r="A278" t="s">
         <v>140</v>
       </c>
@@ -7129,7 +7128,7 @@
         <v>551439040418</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1">
+    <row r="279" spans="1:6">
       <c r="A279" t="s">
         <v>140</v>
       </c>
@@ -7149,7 +7148,7 @@
         <v>549935960334</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1">
+    <row r="280" spans="1:6">
       <c r="A280" t="s">
         <v>140</v>
       </c>
@@ -7169,7 +7168,7 @@
         <v>550049775672</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1">
+    <row r="281" spans="1:6">
       <c r="A281" t="s">
         <v>140</v>
       </c>
@@ -7189,7 +7188,7 @@
         <v>549991133910</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1">
+    <row r="282" spans="1:6">
       <c r="A282" t="s">
         <v>140</v>
       </c>
@@ -7209,7 +7208,7 @@
         <v>558939033824</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1">
+    <row r="283" spans="1:6">
       <c r="A283" t="s">
         <v>140</v>
       </c>
@@ -7229,7 +7228,7 @@
         <v>559058855691</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1">
+    <row r="284" spans="1:6">
       <c r="A284" t="s">
         <v>140</v>
       </c>
@@ -7249,7 +7248,7 @@
         <v>538168745647</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1">
+    <row r="285" spans="1:6">
       <c r="A285" t="s">
         <v>140</v>
       </c>
@@ -7269,7 +7268,7 @@
         <v>559060107295</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1">
+    <row r="286" spans="1:6">
       <c r="A286" t="s">
         <v>140</v>
       </c>
@@ -7289,7 +7288,7 @@
         <v>559061067475</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1">
+    <row r="287" spans="1:6">
       <c r="A287" t="s">
         <v>140</v>
       </c>
@@ -7309,7 +7308,7 @@
         <v>559057139342</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1">
+    <row r="288" spans="1:6">
       <c r="A288" t="s">
         <v>140</v>
       </c>
@@ -7329,7 +7328,7 @@
         <v>535979879291</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1">
+    <row r="289" spans="1:6">
       <c r="A289" t="s">
         <v>140</v>
       </c>
@@ -7349,7 +7348,7 @@
         <v>558927787922</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1">
+    <row r="290" spans="1:6">
       <c r="A290" t="s">
         <v>140</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>558863744021</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1">
+    <row r="291" spans="1:6">
       <c r="A291" t="s">
         <v>140</v>
       </c>
@@ -7389,7 +7388,7 @@
         <v>538049955864</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1">
+    <row r="292" spans="1:6">
       <c r="A292" t="s">
         <v>140</v>
       </c>
@@ -7409,7 +7408,7 @@
         <v>559072843540</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1">
+    <row r="293" spans="1:6">
       <c r="A293" t="s">
         <v>140</v>
       </c>
@@ -7429,7 +7428,7 @@
         <v>560240862759</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1">
+    <row r="294" spans="1:6">
       <c r="A294" t="s">
         <v>140</v>
       </c>
@@ -7449,7 +7448,7 @@
         <v>536050582491</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1">
+    <row r="295" spans="1:6">
       <c r="A295" t="s">
         <v>140</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>558927727575</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1">
+    <row r="296" spans="1:6">
       <c r="A296" t="s">
         <v>140</v>
       </c>
@@ -7489,7 +7488,7 @@
         <v>558991206565</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1">
+    <row r="297" spans="1:6">
       <c r="A297" t="s">
         <v>140</v>
       </c>
@@ -7509,7 +7508,7 @@
         <v>535978323415</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1">
+    <row r="298" spans="1:6">
       <c r="A298" t="s">
         <v>140</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>558861710683</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1">
+    <row r="299" spans="1:6">
       <c r="A299" t="s">
         <v>140</v>
       </c>
@@ -7549,7 +7548,7 @@
         <v>535978299499</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1">
+    <row r="300" spans="1:6">
       <c r="A300" t="s">
         <v>140</v>
       </c>
@@ -7569,7 +7568,7 @@
         <v>559057711673</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1">
+    <row r="301" spans="1:6">
       <c r="A301" t="s">
         <v>140</v>
       </c>
@@ -7589,7 +7588,7 @@
         <v>535978191630</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1">
+    <row r="302" spans="1:6">
       <c r="A302" t="s">
         <v>140</v>
       </c>
@@ -7609,7 +7608,7 @@
         <v>551938397292</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1">
+    <row r="303" spans="1:6">
       <c r="A303" t="s">
         <v>140</v>
       </c>
@@ -7629,7 +7628,7 @@
         <v>551918269493</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1">
+    <row r="304" spans="1:6">
       <c r="A304" t="s">
         <v>140</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>551936745363</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1">
+    <row r="305" spans="1:6">
       <c r="A305" t="s">
         <v>140</v>
       </c>
@@ -7669,7 +7668,7 @@
         <v>529398494706</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1">
+    <row r="306" spans="1:6">
       <c r="A306" t="s">
         <v>140</v>
       </c>
@@ -7789,7 +7788,7 @@
         <v>554456502030</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1">
+    <row r="312" spans="1:6">
       <c r="A312" t="s">
         <v>140</v>
       </c>
@@ -7809,7 +7808,7 @@
         <v>557305798317</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1">
+    <row r="313" spans="1:6">
       <c r="A313" t="s">
         <v>140</v>
       </c>
@@ -7829,7 +7828,7 @@
         <v>557252321309</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1">
+    <row r="314" spans="1:6">
       <c r="A314" t="s">
         <v>140</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>557257361633</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1">
+    <row r="315" spans="1:6">
       <c r="A315" t="s">
         <v>140</v>
       </c>
@@ -7869,7 +7868,7 @@
         <v>559179304670</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1">
+    <row r="316" spans="1:6">
       <c r="A316" t="s">
         <v>140</v>
       </c>
@@ -7889,7 +7888,7 @@
         <v>561025690015</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1">
+    <row r="317" spans="1:6">
       <c r="A317" t="s">
         <v>140</v>
       </c>
@@ -7909,7 +7908,7 @@
         <v>561377683672</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1">
+    <row r="318" spans="1:6">
       <c r="A318" t="s">
         <v>140</v>
       </c>
@@ -7929,7 +7928,7 @@
         <v>557250201024</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1">
+    <row r="319" spans="1:6">
       <c r="A319" t="s">
         <v>140</v>
       </c>
@@ -7949,7 +7948,7 @@
         <v>557304826984</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1">
+    <row r="320" spans="1:6">
       <c r="A320" t="s">
         <v>140</v>
       </c>
@@ -7969,7 +7968,7 @@
         <v>520500394065</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1">
+    <row r="321" spans="1:6">
       <c r="A321" t="s">
         <v>140</v>
       </c>
@@ -7989,7 +7988,7 @@
         <v>536777966001</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1">
+    <row r="322" spans="1:6">
       <c r="A322" t="s">
         <v>140</v>
       </c>
@@ -8009,7 +8008,7 @@
         <v>557297066706</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1">
+    <row r="323" spans="1:6">
       <c r="A323" t="s">
         <v>140</v>
       </c>
@@ -8029,7 +8028,7 @@
         <v>557171392559</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1">
+    <row r="324" spans="1:6">
       <c r="A324" t="s">
         <v>140</v>
       </c>
@@ -8049,7 +8048,7 @@
         <v>557303902515</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1">
+    <row r="325" spans="1:6">
       <c r="A325" t="s">
         <v>140</v>
       </c>
@@ -8069,7 +8068,7 @@
         <v>559269241736</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1">
+    <row r="326" spans="1:6">
       <c r="A326" t="s">
         <v>140</v>
       </c>
@@ -8089,7 +8088,7 @@
         <v>557165008970</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1">
+    <row r="327" spans="1:6">
       <c r="A327" t="s">
         <v>140</v>
       </c>
@@ -8109,7 +8108,7 @@
         <v>520499954937</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1">
+    <row r="328" spans="1:6">
       <c r="A328" t="s">
         <v>140</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>557298018125</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1">
+    <row r="329" spans="1:6">
       <c r="A329" t="s">
         <v>140</v>
       </c>
@@ -8149,7 +8148,7 @@
         <v>557362839334</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1">
+    <row r="330" spans="1:6">
       <c r="A330" t="s">
         <v>140</v>
       </c>
@@ -8169,7 +8168,7 @@
         <v>536741860116</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1">
+    <row r="331" spans="1:6">
       <c r="A331" t="s">
         <v>140</v>
       </c>
@@ -8189,7 +8188,7 @@
         <v>557173516352</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1">
+    <row r="332" spans="1:6">
       <c r="A332" t="s">
         <v>140</v>
       </c>
@@ -8209,7 +8208,7 @@
         <v>14023444768</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1">
+    <row r="333" spans="1:6">
       <c r="A333" t="s">
         <v>140</v>
       </c>
@@ -8229,7 +8228,7 @@
         <v>536996140783</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1">
+    <row r="334" spans="1:6">
       <c r="A334" t="s">
         <v>140</v>
       </c>
@@ -8249,7 +8248,7 @@
         <v>536847031903</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1">
+    <row r="335" spans="1:6">
       <c r="A335" t="s">
         <v>140</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>520270699637</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1">
+    <row r="336" spans="1:6">
       <c r="A336" t="s">
         <v>140</v>
       </c>
@@ -8289,7 +8288,7 @@
         <v>14023480446</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1">
+    <row r="337" spans="1:6">
       <c r="A337" t="s">
         <v>140</v>
       </c>
@@ -8309,7 +8308,7 @@
         <v>13082654232</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1">
+    <row r="338" spans="1:6">
       <c r="A338" t="s">
         <v>140</v>
       </c>
@@ -8329,7 +8328,7 @@
         <v>522920732025</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1">
+    <row r="339" spans="1:6">
       <c r="A339" t="s">
         <v>140</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>520272996081</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1">
+    <row r="340" spans="1:6">
       <c r="A340" t="s">
         <v>140</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>520270401714</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1">
+    <row r="341" spans="1:6">
       <c r="A341" t="s">
         <v>140</v>
       </c>
@@ -8389,7 +8388,7 @@
         <v>534573615994</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1">
+    <row r="342" spans="1:6">
       <c r="A342" t="s">
         <v>140</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>564080535159</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1">
+    <row r="343" spans="1:6">
       <c r="A343" t="s">
         <v>140</v>
       </c>
@@ -8429,7 +8428,7 @@
         <v>522893959694</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1">
+    <row r="344" spans="1:6">
       <c r="A344" t="s">
         <v>140</v>
       </c>
@@ -8449,7 +8448,7 @@
         <v>520272726233</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1">
+    <row r="345" spans="1:6">
       <c r="A345" t="s">
         <v>140</v>
       </c>
@@ -8469,7 +8468,7 @@
         <v>14023436964</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1">
+    <row r="346" spans="1:6">
       <c r="A346" t="s">
         <v>140</v>
       </c>
@@ -8489,7 +8488,7 @@
         <v>536847315304</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1">
+    <row r="347" spans="1:6">
       <c r="A347" t="s">
         <v>140</v>
       </c>
@@ -8509,7 +8508,7 @@
         <v>563946821989</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1">
+    <row r="348" spans="1:6">
       <c r="A348" t="s">
         <v>140</v>
       </c>
@@ -8529,7 +8528,7 @@
         <v>564104944588</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1">
+    <row r="349" spans="1:6">
       <c r="A349" t="s">
         <v>140</v>
       </c>
@@ -8549,7 +8548,7 @@
         <v>534574151394</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1">
+    <row r="350" spans="1:6">
       <c r="A350" t="s">
         <v>140</v>
       </c>
@@ -8569,7 +8568,7 @@
         <v>539027931957</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1">
+    <row r="351" spans="1:6">
       <c r="A351" t="s">
         <v>140</v>
       </c>
@@ -8589,7 +8588,7 @@
         <v>520273012067</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1">
+    <row r="352" spans="1:6">
       <c r="A352" t="s">
         <v>140</v>
       </c>
@@ -8609,7 +8608,7 @@
         <v>563948033154</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1">
+    <row r="353" spans="1:6">
       <c r="A353" t="s">
         <v>140</v>
       </c>
@@ -8629,7 +8628,7 @@
         <v>536957937847</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1">
+    <row r="354" spans="1:6">
       <c r="A354" t="s">
         <v>140</v>
       </c>
@@ -8649,7 +8648,7 @@
         <v>536920910593</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1">
+    <row r="355" spans="1:6">
       <c r="A355" t="s">
         <v>140</v>
       </c>
@@ -8669,7 +8668,7 @@
         <v>552294913080</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1">
+    <row r="356" spans="1:6">
       <c r="A356" t="s">
         <v>140</v>
       </c>
@@ -8689,7 +8688,7 @@
         <v>540290207969</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1">
+    <row r="357" spans="1:6">
       <c r="A357" t="s">
         <v>140</v>
       </c>
@@ -8709,7 +8708,7 @@
         <v>540283992485</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1">
+    <row r="358" spans="1:6">
       <c r="A358" t="s">
         <v>140</v>
       </c>
@@ -8729,7 +8728,7 @@
         <v>536695972182</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1">
+    <row r="359" spans="1:6">
       <c r="A359" t="s">
         <v>140</v>
       </c>
@@ -8749,7 +8748,7 @@
         <v>536847011852</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1">
+    <row r="360" spans="1:6">
       <c r="A360" t="s">
         <v>140</v>
       </c>
@@ -8769,7 +8768,7 @@
         <v>536847235462</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1">
+    <row r="361" spans="1:6">
       <c r="A361" t="s">
         <v>140</v>
       </c>
@@ -8789,7 +8788,7 @@
         <v>552329550911</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1">
+    <row r="362" spans="1:6">
       <c r="A362" t="s">
         <v>140</v>
       </c>
@@ -8809,7 +8808,7 @@
         <v>536847243435</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1">
+    <row r="363" spans="1:6">
       <c r="A363" t="s">
         <v>140</v>
       </c>
@@ -8829,7 +8828,7 @@
         <v>536610825986</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1">
+    <row r="364" spans="1:6">
       <c r="A364" t="s">
         <v>140</v>
       </c>
@@ -8849,7 +8848,7 @@
         <v>536349658964</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1">
+    <row r="365" spans="1:6">
       <c r="A365" t="s">
         <v>140</v>
       </c>
@@ -8870,13 +8869,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F365">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="MOM"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F365"/>
   <conditionalFormatting sqref="F2 E1:E1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>

</xml_diff>